<commit_message>
excel sheet generation and invoice generation done
</commit_message>
<xml_diff>
--- a/order.xlsx
+++ b/order.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="25">
   <si>
     <t>S.no</t>
   </si>
@@ -37,13 +37,52 @@
     <t>Pending</t>
   </si>
   <si>
+    <t>Ayush Saini</t>
+  </si>
+  <si>
+    <t>Processing</t>
+  </si>
+  <si>
+    <t>Payment Done</t>
+  </si>
+  <si>
+    <t>Shipped</t>
+  </si>
+  <si>
+    <t>Tushar Srivastav</t>
+  </si>
+  <si>
+    <t>Out for delivery</t>
+  </si>
+  <si>
     <t>Diksha</t>
   </si>
   <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>Ritika</t>
+  </si>
+  <si>
+    <t>Delivered</t>
+  </si>
+  <si>
+    <t>Abhishek</t>
+  </si>
+  <si>
+    <t>Adarsh</t>
+  </si>
+  <si>
+    <t>Not Done</t>
+  </si>
+  <si>
+    <t>Ankit Upadhyay</t>
+  </si>
+  <si>
     <t>Sumit Sain</t>
   </si>
   <si>
-    <t>Payment Done</t>
+    <t>Amit Kumar</t>
   </si>
   <si>
     <t>Prashant Sharma</t>
@@ -427,7 +466,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E31"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
@@ -495,13 +534,13 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E4">
-        <v>215.45</v>
+        <v>4219.42</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -509,16 +548,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
       <c r="E5">
-        <v>3558.09</v>
+        <v>587.7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -526,16 +565,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E6">
-        <v>1495.77</v>
+        <v>474.22</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -543,15 +582,423 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>581.72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>1601.29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>959.33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>758.73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
         <v>6</v>
       </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7">
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11">
+        <v>215.45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <v>160.95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>128.45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <v>515.02</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15">
+        <v>1455.93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16">
+        <v>1343.86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17">
+        <v>1398.86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18">
+        <v>2202.86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19">
+        <v>379.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20">
+        <v>1251.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21">
+        <v>845.95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22">
+        <v>394.93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23">
+        <v>420.95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24">
+        <v>2755.5699999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25">
+        <v>2061.35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26">
+        <v>3558.09</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27">
+        <v>1495.77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28">
+        <v>1563.69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29">
+        <v>513.73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30">
+        <v>918.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31">
         <v>1878.79</v>
       </c>
     </row>

</xml_diff>

<commit_message>
order stats added in admin panel using charts
</commit_message>
<xml_diff>
--- a/order.xlsx
+++ b/order.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="26">
   <si>
     <t>S.no</t>
   </si>
@@ -34,18 +34,36 @@
     <t>Not Process</t>
   </si>
   <si>
+    <t>Payment Done</t>
+  </si>
+  <si>
+    <t>Abhishek</t>
+  </si>
+  <si>
+    <t>Refunded</t>
+  </si>
+  <si>
+    <t>Diksha</t>
+  </si>
+  <si>
+    <t>Sumit Sain</t>
+  </si>
+  <si>
+    <t>Prashant Sharma</t>
+  </si>
+  <si>
+    <t>Amit Kumar</t>
+  </si>
+  <si>
+    <t>Processing</t>
+  </si>
+  <si>
     <t>Pending</t>
   </si>
   <si>
     <t>Ayush Saini</t>
   </si>
   <si>
-    <t>Processing</t>
-  </si>
-  <si>
-    <t>Payment Done</t>
-  </si>
-  <si>
     <t>Shipped</t>
   </si>
   <si>
@@ -55,9 +73,6 @@
     <t>Out for delivery</t>
   </si>
   <si>
-    <t>Diksha</t>
-  </si>
-  <si>
     <t>Cancelled</t>
   </si>
   <si>
@@ -67,9 +82,6 @@
     <t>Delivered</t>
   </si>
   <si>
-    <t>Abhishek</t>
-  </si>
-  <si>
     <t>Adarsh</t>
   </si>
   <si>
@@ -77,15 +89,6 @@
   </si>
   <si>
     <t>Ankit Upadhyay</t>
-  </si>
-  <si>
-    <t>Sumit Sain</t>
-  </si>
-  <si>
-    <t>Amit Kumar</t>
-  </si>
-  <si>
-    <t>Prashant Sharma</t>
   </si>
 </sst>
 </file>
@@ -466,7 +469,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E63"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
@@ -506,7 +509,7 @@
         <v>7</v>
       </c>
       <c r="E2">
-        <v>4104.09</v>
+        <v>340.95</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -514,16 +517,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E3">
-        <v>4004.09</v>
+        <v>203.45</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -534,13 +537,13 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E4">
-        <v>4219.42</v>
+        <v>2611.67</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -551,13 +554,13 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E5">
-        <v>587.7</v>
+        <v>2311.67</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -568,13 +571,13 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6">
-        <v>474.22</v>
+        <v>790.56</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -582,16 +585,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7">
-        <v>581.72</v>
+        <v>5103.52</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -599,16 +602,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8">
-        <v>1601.29</v>
+        <v>746.7</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -616,16 +619,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E9">
-        <v>959.33</v>
+        <v>609.2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -633,16 +636,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E10">
-        <v>758.73</v>
+        <v>1009.07</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -650,7 +653,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -659,7 +662,7 @@
         <v>7</v>
       </c>
       <c r="E11">
-        <v>215.45</v>
+        <v>891.19</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -667,16 +670,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E12">
-        <v>160.95</v>
+        <v>223.52</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -684,16 +687,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E13">
-        <v>128.45</v>
+        <v>126.95</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -701,16 +704,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E14">
-        <v>515.02</v>
+        <v>120.95</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -718,16 +721,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E15">
-        <v>1455.93</v>
+        <v>553.73</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -735,16 +738,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E16">
-        <v>1343.86</v>
+        <v>645.02</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -752,16 +755,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E17">
-        <v>1398.86</v>
+        <v>1172.67</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -769,16 +772,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E18">
-        <v>2202.86</v>
+        <v>225.95</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -786,16 +789,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E19">
-        <v>379.7</v>
+        <v>116.95</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -803,16 +806,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E20">
-        <v>1251.7</v>
+        <v>128.45</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -820,16 +823,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E21">
-        <v>845.95</v>
+        <v>878.75</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -837,16 +840,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E22">
-        <v>394.93</v>
+        <v>168.35</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -854,16 +857,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E23">
-        <v>420.95</v>
+        <v>1583.74</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -871,16 +874,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E24">
-        <v>2755.5699999999997</v>
+        <v>1865.06</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -888,16 +891,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E25">
-        <v>2061.35</v>
+        <v>554.76</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -905,16 +908,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
       </c>
       <c r="D26" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E26">
-        <v>3558.09</v>
+        <v>1048.75</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -922,7 +925,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
@@ -931,7 +934,7 @@
         <v>7</v>
       </c>
       <c r="E27">
-        <v>1495.77</v>
+        <v>225.95</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -939,16 +942,16 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C28" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E28">
-        <v>1563.69</v>
+        <v>397.7</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -956,16 +959,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E29">
-        <v>513.73</v>
+        <v>628.01</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -973,16 +976,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C30" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E30">
-        <v>918.4</v>
+        <v>542.52</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -990,15 +993,559 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31">
+        <v>542.52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32">
+        <v>150.95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33">
+        <v>150.95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34">
+        <v>4104.09</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35">
+        <v>4004.09</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36">
+        <v>4219.42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37">
+        <v>587.7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38">
+        <v>474.22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39">
+        <v>581.72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40">
+        <v>1601.29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41">
+        <v>959.33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" t="s">
+        <v>20</v>
+      </c>
+      <c r="D42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42">
+        <v>758.73</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
+        <v>15</v>
+      </c>
+      <c r="E43">
+        <v>215.45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44">
+        <v>160.95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" t="s">
+        <v>22</v>
+      </c>
+      <c r="D45" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45">
+        <v>128.45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46">
+        <v>515.02</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" t="s">
+        <v>20</v>
+      </c>
+      <c r="D47" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47">
+        <v>1455.93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" t="s">
+        <v>17</v>
+      </c>
+      <c r="D48" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48">
+        <v>1343.86</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49">
+        <v>1398.86</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" t="s">
+        <v>22</v>
+      </c>
+      <c r="D50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50">
+        <v>2202.86</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51" t="s">
+        <v>20</v>
+      </c>
+      <c r="D51" t="s">
         <v>24</v>
       </c>
-      <c r="C31" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31">
+      <c r="E51">
+        <v>379.7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>23</v>
+      </c>
+      <c r="C52" t="s">
+        <v>20</v>
+      </c>
+      <c r="D52" t="s">
+        <v>20</v>
+      </c>
+      <c r="E52">
+        <v>1251.7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>23</v>
+      </c>
+      <c r="C53" t="s">
+        <v>17</v>
+      </c>
+      <c r="D53" t="s">
+        <v>7</v>
+      </c>
+      <c r="E53">
+        <v>845.95</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>23</v>
+      </c>
+      <c r="C54" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54">
+        <v>394.93</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>21</v>
+      </c>
+      <c r="C55" t="s">
+        <v>22</v>
+      </c>
+      <c r="D55" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55">
+        <v>420.95</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>25</v>
+      </c>
+      <c r="C56" t="s">
+        <v>19</v>
+      </c>
+      <c r="D56" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56">
+        <v>2755.5699999999997</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>25</v>
+      </c>
+      <c r="C57" t="s">
+        <v>19</v>
+      </c>
+      <c r="D57" t="s">
+        <v>7</v>
+      </c>
+      <c r="E57">
+        <v>2061.35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>11</v>
+      </c>
+      <c r="C58" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58">
+        <v>3558.09</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" t="s">
+        <v>15</v>
+      </c>
+      <c r="E59">
+        <v>1495.77</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>11</v>
+      </c>
+      <c r="C60" t="s">
+        <v>19</v>
+      </c>
+      <c r="D60" t="s">
+        <v>7</v>
+      </c>
+      <c r="E60">
+        <v>1563.69</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61" t="s">
+        <v>19</v>
+      </c>
+      <c r="D61" t="s">
+        <v>7</v>
+      </c>
+      <c r="E61">
+        <v>513.73</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>23</v>
+      </c>
+      <c r="C62" t="s">
+        <v>19</v>
+      </c>
+      <c r="D62" t="s">
+        <v>7</v>
+      </c>
+      <c r="E62">
+        <v>918.4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>12</v>
+      </c>
+      <c r="C63" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63" t="s">
+        <v>7</v>
+      </c>
+      <c r="E63">
         <v>1878.79</v>
       </c>
     </row>

</xml_diff>